<commit_message>
Updated sprint backlog with Dimitar's tasks.
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint Backlog/Sprint 2 backlog.xlsx
+++ b/Sprint 2/Sprint Backlog/Sprint 2 backlog.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelwamarema\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dimitar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23460" windowHeight="12975"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Product Backlog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -237,6 +237,12 @@
   </si>
   <si>
     <t>011/02/2020</t>
+  </si>
+  <si>
+    <t>Dimitar</t>
+  </si>
+  <si>
+    <t>Added accesability and text resizing buttons</t>
   </si>
 </sst>
 </file>
@@ -692,9 +698,9 @@
   </sheetPr>
   <dimension ref="A1:AI994"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L23" sqref="L23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2125,8 +2131,38 @@
       <c r="AH25" s="7"/>
       <c r="AI25" s="7"/>
     </row>
-    <row r="26" spans="1:35" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16">
+        <v>4</v>
+      </c>
+      <c r="F26" s="16">
+        <v>6</v>
+      </c>
+      <c r="G26" s="16">
+        <f>F26/E26</f>
+        <v>1.5</v>
+      </c>
+      <c r="H26" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="I26" s="16">
+        <v>4</v>
+      </c>
+      <c r="J26" s="24">
+        <v>43867</v>
+      </c>
+      <c r="K26" s="24">
+        <v>43868</v>
+      </c>
+      <c r="L26" s="16" t="s">
+        <v>26</v>
+      </c>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
@@ -2150,7 +2186,7 @@
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
     </row>
-    <row r="27" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:35" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="N27" s="7"/>
       <c r="O27" s="7"/>
@@ -2302,6 +2338,17 @@
     </row>
     <row r="33" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
       <c r="N33" s="7"/>
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
@@ -2327,6 +2374,17 @@
     </row>
     <row r="34" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
       <c r="N34" s="7"/>
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
@@ -3352,16 +3410,16 @@
     <row r="62" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-      <c r="I62" s="7"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="7"/>
-      <c r="L62" s="7"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
       <c r="M62" s="7"/>
       <c r="N62" s="7"/>
       <c r="O62" s="7"/>
@@ -3389,16 +3447,16 @@
     <row r="63" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+      <c r="I63" s="2"/>
+      <c r="J63" s="2"/>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
       <c r="M63" s="7"/>
       <c r="N63" s="7"/>
       <c r="O63" s="7"/>
@@ -37798,17 +37856,6 @@
     </row>
     <row r="993" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A993" s="2"/>
-      <c r="B993" s="2"/>
-      <c r="C993" s="2"/>
-      <c r="D993" s="2"/>
-      <c r="E993" s="2"/>
-      <c r="F993" s="2"/>
-      <c r="G993" s="2"/>
-      <c r="H993" s="2"/>
-      <c r="I993" s="2"/>
-      <c r="J993" s="2"/>
-      <c r="K993" s="2"/>
-      <c r="L993" s="2"/>
       <c r="M993" s="2"/>
       <c r="N993" s="2"/>
       <c r="O993" s="2"/>
@@ -37835,17 +37882,6 @@
     </row>
     <row r="994" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A994" s="2"/>
-      <c r="B994" s="2"/>
-      <c r="C994" s="2"/>
-      <c r="D994" s="2"/>
-      <c r="E994" s="2"/>
-      <c r="F994" s="2"/>
-      <c r="G994" s="2"/>
-      <c r="H994" s="2"/>
-      <c r="I994" s="2"/>
-      <c r="J994" s="2"/>
-      <c r="K994" s="2"/>
-      <c r="L994" s="2"/>
       <c r="M994" s="2"/>
       <c r="N994" s="2"/>
       <c r="O994" s="2"/>
@@ -37872,11 +37908,11 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L3:L25">
-      <formula1>Status</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showDropDown="1" showErrorMessage="1" sqref="O5:O25">
       <formula1>$A$25</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L3:L26">
+      <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>

</xml_diff>